<commit_message>
Updated the main and pipeline interplay
</commit_message>
<xml_diff>
--- a/ExperimentList/combinations.xlsx
+++ b/ExperimentList/combinations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaspertl/Library/Mobile Documents/com~apple~CloudDocs/Cambridge part III/Project/CompleteCodeGit/ExperimentList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D59C1A4-9811-E74D-A592-4DD549194BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68530EE-8C69-444D-AFEF-04C652C83A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="2180" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="21">
   <si>
     <t>Loss</t>
   </si>
@@ -70,7 +70,19 @@
     <t>MSE</t>
   </si>
   <si>
-    <t>*</t>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>server</t>
+  </si>
+  <si>
+    <t>machine</t>
   </si>
 </sst>
 </file>
@@ -92,7 +104,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +114,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -160,6 +178,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G193"/>
+  <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -473,7 +493,7 @@
     <col min="13" max="13" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,31 +512,48 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5">
-        <v>5</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="G1" s="7"/>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -535,306 +572,406 @@
       <c r="F3" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="5">
-        <v>5</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="G3" s="7"/>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
+        <v>12</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6">
+        <v>12</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="J7">
+        <v>7</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="6">
+        <v>5</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="J8">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2">
+        <v>12</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="J9">
+        <v>9</v>
+      </c>
+      <c r="M9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3">
+        <v>5</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2">
+        <v>12</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="J11">
+        <v>11</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="J12">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2">
+        <v>12</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3">
+        <v>5</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="J14">
+        <v>14</v>
+      </c>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="5">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>15</v>
+      </c>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="3">
+        <v>5</v>
+      </c>
+      <c r="J16">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5">
-        <v>5</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5">
-        <v>2</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="5">
-        <v>5</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="5">
-        <v>5</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="5">
-        <v>2</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="5">
-        <v>5</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="5">
-        <v>5</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="3">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="M16" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="3">
+        <v>12</v>
+      </c>
+      <c r="J17">
+        <v>17</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -853,8 +990,12 @@
       <c r="F18" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>18</v>
+      </c>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -873,8 +1014,14 @@
       <c r="F19" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>19</v>
+      </c>
+      <c r="M19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -893,8 +1040,12 @@
       <c r="F20" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>20</v>
+      </c>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -913,8 +1064,14 @@
       <c r="F21" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>21</v>
+      </c>
+      <c r="M21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -933,28 +1090,35 @@
       <c r="F22" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="4">
-        <v>2</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>22</v>
+      </c>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="5">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="5">
+        <v>12</v>
+      </c>
+      <c r="J23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -973,8 +1137,14 @@
       <c r="F24" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>24</v>
+      </c>
+      <c r="M24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
@@ -993,8 +1163,14 @@
       <c r="F25" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>25</v>
+      </c>
+      <c r="M25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1013,8 +1189,12 @@
       <c r="F26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>26</v>
+      </c>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1033,8 +1213,14 @@
       <c r="F27" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>27</v>
+      </c>
+      <c r="M27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1053,8 +1239,12 @@
       <c r="F28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>28</v>
+      </c>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1073,8 +1263,14 @@
       <c r="F29" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>29</v>
+      </c>
+      <c r="M29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1093,28 +1289,35 @@
       <c r="F30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="4">
-        <v>2</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>30</v>
+      </c>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="5">
+        <v>2</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="5">
+        <v>12</v>
+      </c>
+      <c r="J31">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1133,8 +1336,14 @@
       <c r="F32" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>32</v>
+      </c>
+      <c r="M32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1153,8 +1362,14 @@
       <c r="F33" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>33</v>
+      </c>
+      <c r="M33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1173,8 +1388,11 @@
       <c r="F34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1193,8 +1411,12 @@
       <c r="F35">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>35</v>
+      </c>
+      <c r="M35" s="4"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1213,8 +1435,11 @@
       <c r="F36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1233,8 +1458,12 @@
       <c r="F37">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>37</v>
+      </c>
+      <c r="M37" s="4"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1253,8 +1482,11 @@
       <c r="F38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1273,8 +1505,12 @@
       <c r="F39">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>39</v>
+      </c>
+      <c r="M39" s="4"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1293,8 +1529,11 @@
       <c r="F40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1313,8 +1552,12 @@
       <c r="F41">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>41</v>
+      </c>
+      <c r="M41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1333,8 +1576,11 @@
       <c r="F42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1353,8 +1599,12 @@
       <c r="F43">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>43</v>
+      </c>
+      <c r="M43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1373,8 +1623,11 @@
       <c r="F44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1393,8 +1646,12 @@
       <c r="F45">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>45</v>
+      </c>
+      <c r="M45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1413,8 +1670,11 @@
       <c r="F46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1433,8 +1693,12 @@
       <c r="F47">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>47</v>
+      </c>
+      <c r="M47" s="4"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1453,8 +1717,11 @@
       <c r="F48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J48">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1473,8 +1740,12 @@
       <c r="F49">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J49">
+        <v>49</v>
+      </c>
+      <c r="M49" s="4"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1494,7 +1765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1514,7 +1785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1534,7 +1805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1554,7 +1825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1574,7 +1845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1594,7 +1865,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1614,7 +1885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1634,7 +1905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1654,7 +1925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -1674,7 +1945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -1694,7 +1965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -1714,7 +1985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -1734,7 +2005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -1754,7 +2025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Updated pipeline to automatically run the diffrent sparcities.
</commit_message>
<xml_diff>
--- a/ExperimentList/combinations.xlsx
+++ b/ExperimentList/combinations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaspertl/Library/Mobile Documents/com~apple~CloudDocs/Cambridge part III/Project/CompleteCodeGit/ExperimentList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68530EE-8C69-444D-AFEF-04C652C83A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A99ECE-AF90-C845-B522-57E6829110F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="2180" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="22">
   <si>
     <t>Loss</t>
   </si>
@@ -84,6 +84,9 @@
   <si>
     <t>machine</t>
   </si>
+  <si>
+    <t>s</t>
+  </si>
 </sst>
 </file>
 
@@ -104,7 +107,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,12 +123,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -178,7 +175,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -484,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="R42" sqref="R42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K108" sqref="K108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -512,7 +508,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="6"/>
       <c r="J1">
         <v>1</v>
       </c>
@@ -527,25 +523,25 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6">
-        <v>2</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6">
-        <v>5</v>
-      </c>
-      <c r="G2" s="7"/>
+      <c r="F2" s="5">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6"/>
       <c r="J2">
         <v>2</v>
       </c>
@@ -572,7 +568,7 @@
       <c r="F3" s="2">
         <v>12</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="6"/>
       <c r="J3">
         <v>3</v>
       </c>
@@ -581,25 +577,25 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="6">
-        <v>2</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6">
-        <v>5</v>
-      </c>
-      <c r="G4" s="7"/>
+      <c r="F4" s="5">
+        <v>5</v>
+      </c>
+      <c r="G4" s="6"/>
       <c r="J4">
         <v>4</v>
       </c>
@@ -629,7 +625,7 @@
       <c r="F5" s="2">
         <v>12</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="6"/>
       <c r="J5">
         <v>5</v>
       </c>
@@ -638,25 +634,25 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6">
-        <v>5</v>
-      </c>
-      <c r="G6" s="7"/>
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6"/>
       <c r="J6">
         <v>6</v>
       </c>
@@ -668,25 +664,25 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6">
-        <v>2</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="6">
-        <v>12</v>
-      </c>
-      <c r="G7" s="7"/>
+      <c r="F7" s="5">
+        <v>12</v>
+      </c>
+      <c r="G7" s="6"/>
       <c r="J7">
         <v>7</v>
       </c>
@@ -695,25 +691,25 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="6">
-        <v>5</v>
-      </c>
-      <c r="G8" s="7"/>
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6"/>
       <c r="J8">
         <v>8</v>
       </c>
@@ -743,7 +739,7 @@
       <c r="F9" s="2">
         <v>12</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="6"/>
       <c r="J9">
         <v>9</v>
       </c>
@@ -770,14 +766,14 @@
       <c r="F10" s="3">
         <v>5</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="6"/>
       <c r="J10">
         <v>10</v>
       </c>
       <c r="K10" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -800,11 +796,11 @@
       <c r="F11" s="2">
         <v>12</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="6"/>
       <c r="J11">
         <v>11</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -827,14 +823,14 @@
       <c r="F12" s="3">
         <v>5</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="6"/>
       <c r="J12">
         <v>12</v>
       </c>
       <c r="K12" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="M12" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -857,11 +853,11 @@
       <c r="F13" s="2">
         <v>12</v>
       </c>
-      <c r="G13" s="7"/>
+      <c r="G13" s="6"/>
       <c r="J13">
         <v>13</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -884,40 +880,40 @@
       <c r="F14" s="3">
         <v>5</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="6"/>
       <c r="J14">
         <v>14</v>
       </c>
       <c r="K14" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="M14" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="5">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>12</v>
       </c>
       <c r="J15">
         <v>15</v>
       </c>
-      <c r="M15" s="7"/>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -941,7 +937,7 @@
       <c r="J16">
         <v>16</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="M16" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -967,7 +963,7 @@
       <c r="J17">
         <v>17</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="M17" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -993,7 +989,9 @@
       <c r="J18">
         <v>18</v>
       </c>
-      <c r="M18" s="4"/>
+      <c r="M18" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -1043,7 +1041,9 @@
       <c r="J20">
         <v>20</v>
       </c>
-      <c r="M20" s="4"/>
+      <c r="M20" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -1093,25 +1093,27 @@
       <c r="J22">
         <v>22</v>
       </c>
-      <c r="M22" s="4"/>
+      <c r="M22" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="5">
-        <v>2</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>12</v>
       </c>
       <c r="J23">
@@ -1192,7 +1194,9 @@
       <c r="J26">
         <v>26</v>
       </c>
-      <c r="M26" s="4"/>
+      <c r="M26" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -1242,7 +1246,9 @@
       <c r="J28">
         <v>28</v>
       </c>
-      <c r="M28" s="4"/>
+      <c r="M28" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -1292,25 +1298,27 @@
       <c r="J30">
         <v>30</v>
       </c>
-      <c r="M30" s="4"/>
+      <c r="M30" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="5">
-        <v>2</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="A31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="4">
         <v>12</v>
       </c>
       <c r="J31">
@@ -1414,7 +1422,9 @@
       <c r="J35">
         <v>35</v>
       </c>
-      <c r="M35" s="4"/>
+      <c r="M35" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -1461,7 +1471,9 @@
       <c r="J37">
         <v>37</v>
       </c>
-      <c r="M37" s="4"/>
+      <c r="M37" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -1508,7 +1520,9 @@
       <c r="J39">
         <v>39</v>
       </c>
-      <c r="M39" s="4"/>
+      <c r="M39" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -1555,7 +1569,9 @@
       <c r="J41">
         <v>41</v>
       </c>
-      <c r="M41" s="4"/>
+      <c r="M41" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -1602,7 +1618,9 @@
       <c r="J43">
         <v>43</v>
       </c>
-      <c r="M43" s="4"/>
+      <c r="M43" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -1649,7 +1667,9 @@
       <c r="J45">
         <v>45</v>
       </c>
-      <c r="M45" s="4"/>
+      <c r="M45" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -1696,7 +1716,9 @@
       <c r="J47">
         <v>47</v>
       </c>
-      <c r="M47" s="4"/>
+      <c r="M47" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -1743,7 +1765,9 @@
       <c r="J49">
         <v>49</v>
       </c>
-      <c r="M49" s="4"/>
+      <c r="M49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -1764,6 +1788,9 @@
       <c r="F50">
         <v>5</v>
       </c>
+      <c r="J50">
+        <v>50</v>
+      </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -1784,6 +1811,12 @@
       <c r="F51">
         <v>12</v>
       </c>
+      <c r="J51">
+        <v>51</v>
+      </c>
+      <c r="M51" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -1804,6 +1837,9 @@
       <c r="F52">
         <v>5</v>
       </c>
+      <c r="J52">
+        <v>52</v>
+      </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
@@ -1824,6 +1860,12 @@
       <c r="F53">
         <v>12</v>
       </c>
+      <c r="J53">
+        <v>53</v>
+      </c>
+      <c r="M53" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -1844,6 +1886,9 @@
       <c r="F54">
         <v>5</v>
       </c>
+      <c r="J54">
+        <v>54</v>
+      </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -1864,6 +1909,12 @@
       <c r="F55">
         <v>12</v>
       </c>
+      <c r="J55">
+        <v>55</v>
+      </c>
+      <c r="M55" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
@@ -1884,6 +1935,9 @@
       <c r="F56">
         <v>5</v>
       </c>
+      <c r="J56">
+        <v>56</v>
+      </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -1904,6 +1958,12 @@
       <c r="F57">
         <v>12</v>
       </c>
+      <c r="J57">
+        <v>57</v>
+      </c>
+      <c r="M57" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
@@ -1924,6 +1984,9 @@
       <c r="F58">
         <v>5</v>
       </c>
+      <c r="J58">
+        <v>58</v>
+      </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -1944,6 +2007,12 @@
       <c r="F59">
         <v>12</v>
       </c>
+      <c r="J59">
+        <v>59</v>
+      </c>
+      <c r="M59" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
@@ -1964,6 +2033,9 @@
       <c r="F60">
         <v>5</v>
       </c>
+      <c r="J60">
+        <v>60</v>
+      </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
@@ -1984,6 +2056,12 @@
       <c r="F61">
         <v>12</v>
       </c>
+      <c r="J61">
+        <v>61</v>
+      </c>
+      <c r="M61" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -2004,6 +2082,9 @@
       <c r="F62">
         <v>5</v>
       </c>
+      <c r="J62">
+        <v>62</v>
+      </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
@@ -2024,6 +2105,12 @@
       <c r="F63">
         <v>12</v>
       </c>
+      <c r="J63">
+        <v>63</v>
+      </c>
+      <c r="M63" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
@@ -2044,8 +2131,11 @@
       <c r="F64">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J64">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -2064,8 +2154,14 @@
       <c r="F65">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J65">
+        <v>65</v>
+      </c>
+      <c r="M65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -2084,8 +2180,11 @@
       <c r="F66">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J66">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2104,8 +2203,14 @@
       <c r="F67">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J67">
+        <v>67</v>
+      </c>
+      <c r="M67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2124,8 +2229,11 @@
       <c r="F68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J68">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2144,8 +2252,14 @@
       <c r="F69">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J69">
+        <v>69</v>
+      </c>
+      <c r="M69" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -2164,8 +2278,11 @@
       <c r="F70">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J70">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -2184,8 +2301,14 @@
       <c r="F71">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J71">
+        <v>71</v>
+      </c>
+      <c r="M71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2204,8 +2327,11 @@
       <c r="F72">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J72">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2224,8 +2350,14 @@
       <c r="F73">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J73">
+        <v>73</v>
+      </c>
+      <c r="M73" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2244,8 +2376,11 @@
       <c r="F74">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J74">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2264,8 +2399,14 @@
       <c r="F75">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J75">
+        <v>75</v>
+      </c>
+      <c r="M75" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2284,8 +2425,11 @@
       <c r="F76">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J76">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2304,8 +2448,14 @@
       <c r="F77">
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J77">
+        <v>77</v>
+      </c>
+      <c r="M77" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2324,8 +2474,11 @@
       <c r="F78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J78">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2344,8 +2497,14 @@
       <c r="F79">
         <v>12</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J79">
+        <v>79</v>
+      </c>
+      <c r="M79" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2364,8 +2523,11 @@
       <c r="F80">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J80">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2384,8 +2546,14 @@
       <c r="F81">
         <v>12</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J81">
+        <v>81</v>
+      </c>
+      <c r="M81" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2404,8 +2572,11 @@
       <c r="F82">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J82">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -2424,8 +2595,14 @@
       <c r="F83">
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J83">
+        <v>83</v>
+      </c>
+      <c r="M83" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2444,8 +2621,11 @@
       <c r="F84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J84">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2464,8 +2644,14 @@
       <c r="F85">
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J85">
+        <v>85</v>
+      </c>
+      <c r="M85" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2484,8 +2670,11 @@
       <c r="F86">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J86">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -2504,8 +2693,14 @@
       <c r="F87">
         <v>12</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J87">
+        <v>87</v>
+      </c>
+      <c r="M87" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2524,8 +2719,11 @@
       <c r="F88">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J88">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2544,8 +2742,14 @@
       <c r="F89">
         <v>12</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J89">
+        <v>89</v>
+      </c>
+      <c r="M89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2564,8 +2768,11 @@
       <c r="F90">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J90">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2584,8 +2791,14 @@
       <c r="F91">
         <v>12</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J91">
+        <v>91</v>
+      </c>
+      <c r="M91" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2604,8 +2817,11 @@
       <c r="F92">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J92">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -2624,8 +2840,14 @@
       <c r="F93">
         <v>12</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J93">
+        <v>93</v>
+      </c>
+      <c r="M93" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -2644,8 +2866,11 @@
       <c r="F94">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J94">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2664,8 +2889,14 @@
       <c r="F95">
         <v>12</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J95">
+        <v>95</v>
+      </c>
+      <c r="M95" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2684,8 +2915,11 @@
       <c r="F96">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J96">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -2704,8 +2938,14 @@
       <c r="F97">
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J97">
+        <v>97</v>
+      </c>
+      <c r="M97" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -2725,7 +2965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>15</v>
       </c>
@@ -2745,7 +2985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -2765,7 +3005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -2785,7 +3025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>15</v>
       </c>
@@ -2805,7 +3045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>15</v>
       </c>
@@ -2825,7 +3065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -2845,7 +3085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>15</v>
       </c>
@@ -2865,7 +3105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>15</v>
       </c>
@@ -2885,7 +3125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>15</v>
       </c>
@@ -2905,7 +3145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>15</v>
       </c>
@@ -2925,7 +3165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>15</v>
       </c>
@@ -2945,7 +3185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>15</v>
       </c>
@@ -2965,7 +3205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>15</v>
       </c>
@@ -2985,7 +3225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Small updates to pipeline (sparsity)
</commit_message>
<xml_diff>
--- a/ExperimentList/combinations.xlsx
+++ b/ExperimentList/combinations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaspertl/Library/Mobile Documents/com~apple~CloudDocs/Cambridge part III/Project/CompleteCodeGit/ExperimentList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A99ECE-AF90-C845-B522-57E6829110F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFE8235-9005-6A4B-ADDD-63062E768CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K108" sqref="K108"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="Q79" sqref="Q79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2746,7 +2746,7 @@
         <v>89</v>
       </c>
       <c r="M89" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
@@ -2795,7 +2795,7 @@
         <v>91</v>
       </c>
       <c r="M91" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
@@ -2844,7 +2844,7 @@
         <v>93</v>
       </c>
       <c r="M93" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -2893,7 +2893,7 @@
         <v>95</v>
       </c>
       <c r="M95" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -2942,7 +2942,7 @@
         <v>97</v>
       </c>
       <c r="M97" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
All emlements function so that we can get one of the figures for generalized pooling
</commit_message>
<xml_diff>
--- a/ExperimentList/combinations.xlsx
+++ b/ExperimentList/combinations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaspertl/Library/Mobile Documents/com~apple~CloudDocs/Cambridge part III/Project/CompleteCodeGit/ExperimentList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571AFEF9-28D4-5045-9CBA-9E1E4E0B3B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B884A0BE-97DA-734E-8C4F-4A397612B10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5060" yWindow="900" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="23">
   <si>
     <t>Loss</t>
   </si>
@@ -180,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -189,8 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -495,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M151"/>
+  <dimension ref="A1:M156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="F150" sqref="F150:F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -525,7 +524,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J1">
@@ -560,7 +559,6 @@
       <c r="F2" s="5">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
       <c r="J2">
         <v>2</v>
       </c>
@@ -587,7 +585,6 @@
       <c r="F3" s="2">
         <v>12</v>
       </c>
-      <c r="G3" s="6"/>
       <c r="J3">
         <v>3</v>
       </c>
@@ -614,7 +611,6 @@
       <c r="F4" s="5">
         <v>5</v>
       </c>
-      <c r="G4" s="6"/>
       <c r="J4">
         <v>4</v>
       </c>
@@ -644,7 +640,6 @@
       <c r="F5" s="2">
         <v>12</v>
       </c>
-      <c r="G5" s="6"/>
       <c r="J5">
         <v>5</v>
       </c>
@@ -671,7 +666,6 @@
       <c r="F6" s="5">
         <v>5</v>
       </c>
-      <c r="G6" s="6"/>
       <c r="J6">
         <v>6</v>
       </c>
@@ -701,7 +695,6 @@
       <c r="F7" s="5">
         <v>12</v>
       </c>
-      <c r="G7" s="6"/>
       <c r="J7">
         <v>7</v>
       </c>
@@ -728,7 +721,6 @@
       <c r="F8" s="5">
         <v>5</v>
       </c>
-      <c r="G8" s="6"/>
       <c r="J8">
         <v>8</v>
       </c>
@@ -758,7 +750,6 @@
       <c r="F9" s="2">
         <v>12</v>
       </c>
-      <c r="G9" s="6"/>
       <c r="J9">
         <v>9</v>
       </c>
@@ -785,14 +776,13 @@
       <c r="F10" s="3">
         <v>5</v>
       </c>
-      <c r="G10" s="6"/>
       <c r="J10">
         <v>10</v>
       </c>
       <c r="K10" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -815,11 +805,10 @@
       <c r="F11" s="2">
         <v>12</v>
       </c>
-      <c r="G11" s="6"/>
       <c r="J11">
         <v>11</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="M11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -842,14 +831,13 @@
       <c r="F12" s="3">
         <v>5</v>
       </c>
-      <c r="G12" s="6"/>
       <c r="J12">
         <v>12</v>
       </c>
       <c r="K12" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -872,11 +860,10 @@
       <c r="F13" s="2">
         <v>12</v>
       </c>
-      <c r="G13" s="6"/>
       <c r="J13">
         <v>13</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="M13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -899,14 +886,13 @@
       <c r="F14" s="3">
         <v>5</v>
       </c>
-      <c r="G14" s="6"/>
       <c r="J14">
         <v>14</v>
       </c>
       <c r="K14" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="M14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -932,7 +918,6 @@
       <c r="J15">
         <v>15</v>
       </c>
-      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -956,7 +941,7 @@
       <c r="J16">
         <v>16</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="M16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -982,7 +967,7 @@
       <c r="J17">
         <v>17</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1008,7 +993,7 @@
       <c r="J18">
         <v>18</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="M18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1060,7 +1045,7 @@
       <c r="J20">
         <v>20</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="M20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1112,7 +1097,7 @@
       <c r="J22">
         <v>22</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="M22" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1213,7 +1198,7 @@
       <c r="J26">
         <v>26</v>
       </c>
-      <c r="M26" s="6" t="s">
+      <c r="M26" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1265,7 +1250,7 @@
       <c r="J28">
         <v>28</v>
       </c>
-      <c r="M28" s="6" t="s">
+      <c r="M28" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1317,7 +1302,7 @@
       <c r="J30">
         <v>30</v>
       </c>
-      <c r="M30" s="6" t="s">
+      <c r="M30" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1450,7 +1435,7 @@
       <c r="J35">
         <v>35</v>
       </c>
-      <c r="M35" s="6" t="s">
+      <c r="M35" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1508,7 +1493,7 @@
       <c r="J37">
         <v>37</v>
       </c>
-      <c r="M37" s="6" t="s">
+      <c r="M37" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3222,6 +3207,9 @@
       <c r="J108">
         <v>108</v>
       </c>
+      <c r="M108" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
@@ -3248,6 +3236,9 @@
       <c r="J109">
         <v>109</v>
       </c>
+      <c r="M109" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
@@ -3274,6 +3265,9 @@
       <c r="J110">
         <v>110</v>
       </c>
+      <c r="M110" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
@@ -3300,6 +3294,9 @@
       <c r="J111">
         <v>111</v>
       </c>
+      <c r="M111" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
@@ -3326,8 +3323,11 @@
       <c r="J112">
         <v>112</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M112" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -3352,8 +3352,11 @@
       <c r="J113">
         <v>113</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M113" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3378,8 +3381,11 @@
       <c r="J114">
         <v>114</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M114" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3404,8 +3410,11 @@
       <c r="J115">
         <v>115</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M115" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3431,7 +3440,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -3457,7 +3466,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -3483,7 +3492,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3509,7 +3518,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3535,7 +3544,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -3561,7 +3570,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>6</v>
       </c>
@@ -3587,7 +3596,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -3613,7 +3622,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -3639,7 +3648,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>6</v>
       </c>
@@ -3665,7 +3674,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>6</v>
       </c>
@@ -3691,7 +3700,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -3717,7 +3726,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -4211,6 +4220,21 @@
         <v>146</v>
       </c>
     </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J147">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J148">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J149">
+        <v>149</v>
+      </c>
+    </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>6</v>
@@ -4225,7 +4249,7 @@
         <v>21</v>
       </c>
       <c r="E150" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F150">
         <v>5</v>
@@ -4233,6 +4257,9 @@
       <c r="G150">
         <v>1</v>
       </c>
+      <c r="J150">
+        <v>150</v>
+      </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
@@ -4245,13 +4272,149 @@
         <v>14</v>
       </c>
       <c r="D151" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E151" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F151">
         <v>5</v>
+      </c>
+      <c r="G151">
+        <v>2</v>
+      </c>
+      <c r="J151">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>6</v>
+      </c>
+      <c r="B152">
+        <v>2</v>
+      </c>
+      <c r="C152" t="s">
+        <v>14</v>
+      </c>
+      <c r="D152" t="s">
+        <v>21</v>
+      </c>
+      <c r="E152" t="s">
+        <v>10</v>
+      </c>
+      <c r="F152">
+        <v>5</v>
+      </c>
+      <c r="G152">
+        <v>4</v>
+      </c>
+      <c r="J152">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>6</v>
+      </c>
+      <c r="B153">
+        <v>2</v>
+      </c>
+      <c r="C153" t="s">
+        <v>14</v>
+      </c>
+      <c r="D153" t="s">
+        <v>21</v>
+      </c>
+      <c r="E153" t="s">
+        <v>10</v>
+      </c>
+      <c r="F153">
+        <v>5</v>
+      </c>
+      <c r="G153">
+        <v>8</v>
+      </c>
+      <c r="J153">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B154">
+        <v>2</v>
+      </c>
+      <c r="C154" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154" t="s">
+        <v>21</v>
+      </c>
+      <c r="E154" t="s">
+        <v>10</v>
+      </c>
+      <c r="F154">
+        <v>5</v>
+      </c>
+      <c r="G154">
+        <v>16</v>
+      </c>
+      <c r="J154">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>6</v>
+      </c>
+      <c r="B155">
+        <v>2</v>
+      </c>
+      <c r="C155" t="s">
+        <v>14</v>
+      </c>
+      <c r="D155" t="s">
+        <v>21</v>
+      </c>
+      <c r="E155" t="s">
+        <v>10</v>
+      </c>
+      <c r="F155">
+        <v>5</v>
+      </c>
+      <c r="G155">
+        <v>32</v>
+      </c>
+      <c r="J155">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>6</v>
+      </c>
+      <c r="B156">
+        <v>2</v>
+      </c>
+      <c r="C156" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156" t="s">
+        <v>21</v>
+      </c>
+      <c r="E156" t="s">
+        <v>10</v>
+      </c>
+      <c r="F156">
+        <v>5</v>
+      </c>
+      <c r="G156">
+        <v>64</v>
+      </c>
+      <c r="J156">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plotting for basis allignment
</commit_message>
<xml_diff>
--- a/ExperimentList/combinations.xlsx
+++ b/ExperimentList/combinations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaspertl/Library/Mobile Documents/com~apple~CloudDocs/Cambridge part III/Project/CompleteCodeGit/ExperimentList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B884A0BE-97DA-734E-8C4F-4A397612B10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC728E2-06C2-EC43-B8C5-A47300467E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5060" yWindow="900" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="23">
   <si>
     <t>Loss</t>
   </si>
@@ -494,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M156"/>
+  <dimension ref="A1:M160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150:F156"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="M155" sqref="M155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4417,6 +4417,62 @@
         <v>156</v>
       </c>
     </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J157">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J158">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>6</v>
+      </c>
+      <c r="B159">
+        <v>2</v>
+      </c>
+      <c r="C159" t="s">
+        <v>14</v>
+      </c>
+      <c r="D159" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" t="s">
+        <v>12</v>
+      </c>
+      <c r="F159">
+        <v>3</v>
+      </c>
+      <c r="J159">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>6</v>
+      </c>
+      <c r="B160">
+        <v>2</v>
+      </c>
+      <c r="C160" t="s">
+        <v>14</v>
+      </c>
+      <c r="D160" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" t="s">
+        <v>12</v>
+      </c>
+      <c r="F160">
+        <v>4</v>
+      </c>
+      <c r="J160">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to noise functionality
</commit_message>
<xml_diff>
--- a/ExperimentList/combinations.xlsx
+++ b/ExperimentList/combinations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaspertl/Library/Mobile Documents/com~apple~CloudDocs/Cambridge part III/Project/CompleteCodeGit/ExperimentList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3CA81E-6187-A24A-A1A4-AD89DDB7AA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1A3529-FEF1-D94C-871C-FE08BFAA34EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="35">
   <si>
     <t>Loss</t>
   </si>
@@ -536,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M185"/>
+  <dimension ref="A1:M195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="H183" sqref="H183"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="G194" sqref="G194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5000,6 +5000,221 @@
         <v>185</v>
       </c>
     </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J186">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J187">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>6</v>
+      </c>
+      <c r="B188">
+        <v>2</v>
+      </c>
+      <c r="C188" t="s">
+        <v>14</v>
+      </c>
+      <c r="D188" t="s">
+        <v>21</v>
+      </c>
+      <c r="E188" t="s">
+        <v>10</v>
+      </c>
+      <c r="F188">
+        <v>12</v>
+      </c>
+      <c r="G188">
+        <v>1</v>
+      </c>
+      <c r="J188">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>6</v>
+      </c>
+      <c r="B189">
+        <v>2</v>
+      </c>
+      <c r="C189" t="s">
+        <v>14</v>
+      </c>
+      <c r="D189" t="s">
+        <v>21</v>
+      </c>
+      <c r="E189" t="s">
+        <v>10</v>
+      </c>
+      <c r="F189">
+        <v>12</v>
+      </c>
+      <c r="G189">
+        <v>2</v>
+      </c>
+      <c r="J189">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>6</v>
+      </c>
+      <c r="B190">
+        <v>2</v>
+      </c>
+      <c r="C190" t="s">
+        <v>14</v>
+      </c>
+      <c r="D190" t="s">
+        <v>21</v>
+      </c>
+      <c r="E190" t="s">
+        <v>10</v>
+      </c>
+      <c r="F190">
+        <v>12</v>
+      </c>
+      <c r="G190">
+        <v>3</v>
+      </c>
+      <c r="J190">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>6</v>
+      </c>
+      <c r="B191">
+        <v>2</v>
+      </c>
+      <c r="C191" t="s">
+        <v>14</v>
+      </c>
+      <c r="D191" t="s">
+        <v>21</v>
+      </c>
+      <c r="E191" t="s">
+        <v>10</v>
+      </c>
+      <c r="F191">
+        <v>12</v>
+      </c>
+      <c r="G191">
+        <v>4</v>
+      </c>
+      <c r="J191">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>6</v>
+      </c>
+      <c r="B192">
+        <v>2</v>
+      </c>
+      <c r="C192" t="s">
+        <v>14</v>
+      </c>
+      <c r="D192" t="s">
+        <v>21</v>
+      </c>
+      <c r="E192" t="s">
+        <v>10</v>
+      </c>
+      <c r="F192">
+        <v>12</v>
+      </c>
+      <c r="G192">
+        <v>5</v>
+      </c>
+      <c r="J192">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>6</v>
+      </c>
+      <c r="B193">
+        <v>2</v>
+      </c>
+      <c r="C193" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" t="s">
+        <v>21</v>
+      </c>
+      <c r="E193" t="s">
+        <v>10</v>
+      </c>
+      <c r="F193">
+        <v>12</v>
+      </c>
+      <c r="G193">
+        <v>6</v>
+      </c>
+      <c r="J193">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>6</v>
+      </c>
+      <c r="B194">
+        <v>2</v>
+      </c>
+      <c r="C194" t="s">
+        <v>14</v>
+      </c>
+      <c r="D194" t="s">
+        <v>21</v>
+      </c>
+      <c r="E194" t="s">
+        <v>10</v>
+      </c>
+      <c r="F194">
+        <v>12</v>
+      </c>
+      <c r="G194">
+        <v>25</v>
+      </c>
+      <c r="J194">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>6</v>
+      </c>
+      <c r="B195">
+        <v>2</v>
+      </c>
+      <c r="C195" t="s">
+        <v>14</v>
+      </c>
+      <c r="D195" t="s">
+        <v>13</v>
+      </c>
+      <c r="E195" t="s">
+        <v>10</v>
+      </c>
+      <c r="F195">
+        <v>12</v>
+      </c>
+      <c r="J195">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updates to output via PipelineUtils
</commit_message>
<xml_diff>
--- a/ExperimentList/combinations.xlsx
+++ b/ExperimentList/combinations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaspertl/Library/Mobile Documents/com~apple~CloudDocs/Cambridge part III/Project/CompleteCodeGit/ExperimentList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1A3529-FEF1-D94C-871C-FE08BFAA34EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732AA303-2CC3-CD4B-BCB0-F3594312BF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5860" yWindow="1280" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="45">
   <si>
     <t>Loss</t>
   </si>
@@ -125,6 +125,36 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>4, 4, 2</t>
+  </si>
+  <si>
+    <t>6, 6, 4</t>
+  </si>
+  <si>
+    <t>8, 8, 6</t>
+  </si>
+  <si>
+    <t>10, 10, 8</t>
+  </si>
+  <si>
+    <t>12, 12, 10</t>
+  </si>
+  <si>
+    <t>13, 13, 11</t>
+  </si>
+  <si>
+    <t>11, 11, 9</t>
+  </si>
+  <si>
+    <t>9, 9, 7</t>
+  </si>
+  <si>
+    <t>7, 7, 5</t>
+  </si>
+  <si>
+    <t>5, 5, 3</t>
   </si>
 </sst>
 </file>
@@ -536,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M195"/>
+  <dimension ref="A1:M207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="G194" sqref="G194"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="H201" sqref="H201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5215,6 +5245,206 @@
         <v>195</v>
       </c>
     </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>6</v>
+      </c>
+      <c r="B198">
+        <v>2</v>
+      </c>
+      <c r="C198" t="s">
+        <v>7</v>
+      </c>
+      <c r="D198" t="s">
+        <v>8</v>
+      </c>
+      <c r="E198" t="s">
+        <v>23</v>
+      </c>
+      <c r="F198" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>6</v>
+      </c>
+      <c r="B199">
+        <v>2</v>
+      </c>
+      <c r="C199" t="s">
+        <v>7</v>
+      </c>
+      <c r="D199" t="s">
+        <v>8</v>
+      </c>
+      <c r="E199" t="s">
+        <v>23</v>
+      </c>
+      <c r="F199" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>6</v>
+      </c>
+      <c r="B200">
+        <v>2</v>
+      </c>
+      <c r="C200" t="s">
+        <v>7</v>
+      </c>
+      <c r="D200" t="s">
+        <v>8</v>
+      </c>
+      <c r="E200" t="s">
+        <v>23</v>
+      </c>
+      <c r="F200" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>6</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201" t="s">
+        <v>7</v>
+      </c>
+      <c r="D201" t="s">
+        <v>8</v>
+      </c>
+      <c r="E201" t="s">
+        <v>23</v>
+      </c>
+      <c r="F201" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>6</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+      <c r="C202" t="s">
+        <v>7</v>
+      </c>
+      <c r="D202" t="s">
+        <v>8</v>
+      </c>
+      <c r="E202" t="s">
+        <v>23</v>
+      </c>
+      <c r="F202" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>6</v>
+      </c>
+      <c r="B203">
+        <v>2</v>
+      </c>
+      <c r="C203" t="s">
+        <v>7</v>
+      </c>
+      <c r="D203" t="s">
+        <v>8</v>
+      </c>
+      <c r="E203" t="s">
+        <v>23</v>
+      </c>
+      <c r="F203" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>6</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+      <c r="C204" t="s">
+        <v>7</v>
+      </c>
+      <c r="D204" t="s">
+        <v>8</v>
+      </c>
+      <c r="E204" t="s">
+        <v>23</v>
+      </c>
+      <c r="F204" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>6</v>
+      </c>
+      <c r="B205">
+        <v>2</v>
+      </c>
+      <c r="C205" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205" t="s">
+        <v>8</v>
+      </c>
+      <c r="E205" t="s">
+        <v>23</v>
+      </c>
+      <c r="F205" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>6</v>
+      </c>
+      <c r="B206">
+        <v>2</v>
+      </c>
+      <c r="C206" t="s">
+        <v>7</v>
+      </c>
+      <c r="D206" t="s">
+        <v>8</v>
+      </c>
+      <c r="E206" t="s">
+        <v>23</v>
+      </c>
+      <c r="F206" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>6</v>
+      </c>
+      <c r="B207">
+        <v>2</v>
+      </c>
+      <c r="C207" t="s">
+        <v>7</v>
+      </c>
+      <c r="D207" t="s">
+        <v>8</v>
+      </c>
+      <c r="E207" t="s">
+        <v>23</v>
+      </c>
+      <c r="F207" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>